<commit_message>
Dev #268: spec for new tab model
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/single_sheet_table.xlsx
+++ b/spec/fixtures/files/single_sheet_table.xlsx
@@ -8,10 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="census" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Tab" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">census!$A$5:$M$101</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Tab!$A$5:$M$101</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -11857,7 +11857,7 @@
   <dimension ref="A1:M1243"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1235" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11871,7 +11871,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="34.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="18.12"/>

</xml_diff>

<commit_message>
Dev #621 - remove hardcoding
Move from hardcoded tab parsing classes towards a database based set of
regular expressions.
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/single_sheet_table.xlsx
+++ b/spec/fixtures/files/single_sheet_table.xlsx
@@ -8,10 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tab" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="KS4" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Tab!$A$5:$M$101</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KS4!$A$5:$M$101</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -11765,13 +11765,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -11850,17 +11850,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M1243"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1235" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A928" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27"/>
@@ -11869,13 +11869,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="54.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="34.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="3" width="9.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="3" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52882,7 +52882,9 @@
   </sheetData>
   <autoFilter ref="A5:M101"/>
   <conditionalFormatting sqref="L7:L114 L123:L1243">
-    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Yes" dxfId="0"/>
+    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Yes" dxfId="0">
+      <formula>NOT(ISERROR(SEARCH("Yes",L7)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M6 M122" type="list">

</xml_diff>